<commit_message>
Add user file path input & update README
</commit_message>
<xml_diff>
--- a/Bob MD Extraction file.xlsx
+++ b/Bob MD Extraction file.xlsx
@@ -1,84 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdulqadir Abuharrus\Documents\My projects\Dalia PDF Scrape\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1CB60F-0977-4BB0-9FC2-EFD7B6BDB6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="19416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t>Heading Type</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Bob was here</t>
-  </si>
-  <si>
-    <t>Bob's story</t>
-  </si>
-  <si>
-    <t>He loved eating cheeseburgers.  
-When he was 13 he always ate cheeseburgers.  
-He then became 32 and still loved cheeseburgers.</t>
-  </si>
-  <si>
-    <t>We lost Bob!</t>
-  </si>
-  <si>
-    <t>We’ll always miss Bob.</t>
-  </si>
-  <si>
-    <t>Bob’s Legacy</t>
-  </si>
-  <si>
-    <t>Honor Bob</t>
-  </si>
-  <si>
-    <t>We’ll forever honor Bob.  
-The next time you eat cheeseburgers make sure you honor Bob’s memory and always keep him in your thoughts for he was pure of heart and loved cheeseburgers to the very end!</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,46 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,78 +420,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="55.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Headers</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Heading Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bob was here</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bob's story</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>He loved eating cheeseburgers.  
+When he was 13 he always ate cheeseburgers.  
+He then became 32 and still loved cheeseburgers.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>We lost Bob!</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>2</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>We’ll always miss Bob.</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bob’s Legacy</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>1</v>
       </c>
+      <c r="C5" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Honor Bob</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>We’ll forever honor Bob.  
+The next time you eat cheeseburgers make sure you honor Bob’s memory and always keep him in your thoughts for he was pure of heart and loved cheeseburgers to the very end!</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>